<commit_message>
update Core1 and PIO
Pio for encoder services 2 SM machines, updated xls docs
</commit_message>
<xml_diff>
--- a/Block diagram.xlsx
+++ b/Block diagram.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave\Documents\pico-robo-wheels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4D4AC3-BD3B-4D54-B36B-2DA2D9C42215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98055430-6AF1-474D-BFE9-9F96FACF96B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="765" windowWidth="20490" windowHeight="10605" xr2:uid="{991C9B8B-21B3-447E-81C5-65B03554A51A}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="20490" windowHeight="10605" activeTab="1" xr2:uid="{991C9B8B-21B3-447E-81C5-65B03554A51A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,6 +34,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>IRQ relative addressing</t>
+  </si>
+  <si>
+    <t>Two Sm's are running the same code</t>
+  </si>
+  <si>
+    <t>each sm engine must set Two IRQ bits, one for count up, one for count down</t>
+  </si>
+  <si>
+    <t>With 2 sm's that means 4 total IRQ bits in the PIO Block are used</t>
+  </si>
+  <si>
+    <t>Note that these IRQ bits ARE NOT CPU IRQ BITS ( they are mapped to CPU IRQ Bits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO we Map SM=0 IRQ 0,2 ( up,down) to CPU IRQ 0.  then </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO we Map SM=1 IRQ 1,3 ( up,down) to CPU IRQ 1.  then </t>
+  </si>
+  <si>
+    <t>Then each IRQ handler on Core1 must Query the SM interrupt register to figure out wich direction to move position</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1889,6 +1919,1361 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>29430</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>181718</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A47FE4D-3EB9-874B-B16F-32C8DD2A45BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="381000"/>
+          <a:ext cx="6125430" cy="5325218"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E092AEE0-014F-79A0-6F1E-B9A205E7F766}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7762875" y="1933575"/>
+          <a:ext cx="2333625" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8265AD5-4F83-4D23-A206-9AAF2B3CEDD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7781925" y="2266950"/>
+          <a:ext cx="2333625" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFAB121B-3BF3-4D13-99A1-7E84B801B911}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7734300" y="2781300"/>
+          <a:ext cx="2333625" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3528CAD-888C-4A3B-AA01-B9A9DB79F084}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7753350" y="3114675"/>
+          <a:ext cx="2333625" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="684867" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77B261A4-5DB6-F63F-68E1-0C674EC8B2B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10201275" y="1714500"/>
+          <a:ext cx="684867" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>LeftEncA</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="687496" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAE272EF-F56D-4E9D-A840-68E4C8C1CE73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10201275" y="2105025"/>
+          <a:ext cx="687496" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>LeftEncB</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="757580" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55F60BDC-C94E-4509-A00F-1CC61D771EC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10191750" y="2590800"/>
+          <a:ext cx="757580" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>RightEncA</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="760208" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13198139-27CE-4993-8046-236E5396FE6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10182225" y="2914650"/>
+          <a:ext cx="760208" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>RightEncB</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{155055EF-CA19-5645-01DC-0CA6A1C1A000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5800725" y="2457450"/>
+          <a:ext cx="1905000" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1482540B-EB50-4F00-9B32-D2267F606094}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5772150" y="2809875"/>
+          <a:ext cx="1905000" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14B0C1E7-841C-4C34-B16B-F1D7429AF8C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5791200" y="1971675"/>
+          <a:ext cx="1905000" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F7DE76E-7899-4FBA-B580-11E2F8D0647C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5724525" y="1638300"/>
+          <a:ext cx="1905000" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Oval 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29564A6E-4EF1-D181-CE8B-B1212B4A9731}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10067925" y="1581150"/>
+          <a:ext cx="1047750" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Oval 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FBE8104-996A-4437-AADD-F6DA27932992}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10067925" y="2466975"/>
+          <a:ext cx="1047750" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAB65940-BAA6-CF70-0B99-E27593FF4286}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3324225" y="704850"/>
+          <a:ext cx="1914525" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7BA6A2A-413F-4220-AF4F-2477A42E3811}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3143250" y="933450"/>
+          <a:ext cx="1895475" cy="1571625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1295400" cy="676275"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="TextBox 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D4F7CC9-D1CE-B5A3-7EC7-DF24B09B8880}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1190625" y="561975"/>
+          <a:ext cx="1295400" cy="676275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Core</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5289140" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="TextBox 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA9ED32B-EE01-ADFF-D8F5-492A070DB5E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372225" y="857250"/>
+          <a:ext cx="5289140" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Same PIO</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> code runs on both State Machines, but connected to different GPIO and  SM IRQ's</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="421847" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="TextBox 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74EF014D-759C-3A1B-DBDE-EA35607CF9FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="1704975"/>
+          <a:ext cx="421847" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>GP3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="421847" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="TextBox 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AEC1E91-E9A1-43CF-866E-99014D94E1D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8601075" y="2000250"/>
+          <a:ext cx="421847" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>GP4</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="421847" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="TextBox 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F9BE6FA-876C-4619-83A8-5BFD4B712055}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8629650" y="2581275"/>
+          <a:ext cx="421847" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>GP5</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="421847" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="TextBox 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{055D6B81-2B19-4EC5-A8FB-AB70AE689A8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8639175" y="2905125"/>
+          <a:ext cx="421847" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>GP6</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2677977" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="TextBox 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCA2BDD8-5F8F-48D2-976B-1A0B4C4268C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="190500"/>
+          <a:ext cx="2677977" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Core1 services SM IRQ's and keeps Position  </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2211,7 +3596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D3CFB4-6201-4E13-A5FA-28A7E5A461CF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -2220,4 +3605,60 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE9D427-C038-416B-B3CB-C49351CC73FA}">
+  <dimension ref="O20:O27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="20" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add speed calcs to core 1
</commit_message>
<xml_diff>
--- a/Block diagram.xlsx
+++ b/Block diagram.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave\Documents\pico-robo-wheels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98055430-6AF1-474D-BFE9-9F96FACF96B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B90B7F2-FF30-4415-B79A-C8FA7F77C410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="765" windowWidth="20490" windowHeight="10605" activeTab="1" xr2:uid="{991C9B8B-21B3-447E-81C5-65B03554A51A}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="20490" windowHeight="10605" activeTab="3" xr2:uid="{991C9B8B-21B3-447E-81C5-65B03554A51A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Shinlin Motor" sheetId="3" r:id="rId3"/>
+    <sheet name="Encoder calcs" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>IRQ relative addressing</t>
   </si>
@@ -62,11 +64,92 @@
   <si>
     <t>Then each IRQ handler on Core1 must Query the SM interrupt register to figure out wich direction to move position</t>
   </si>
+  <si>
+    <t xml:space="preserve">Shinlin </t>
+  </si>
+  <si>
+    <t>1XYA</t>
+  </si>
+  <si>
+    <t>inches</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>mm diam</t>
+  </si>
+  <si>
+    <t>circumference</t>
+  </si>
+  <si>
+    <t>um diam</t>
+  </si>
+  <si>
+    <t>mm Circum</t>
+  </si>
+  <si>
+    <t>um circ</t>
+  </si>
+  <si>
+    <t>gear ratio</t>
+  </si>
+  <si>
+    <t>cpr</t>
+  </si>
+  <si>
+    <t>encrev/Wheel rev</t>
+  </si>
+  <si>
+    <t>distance per enocder pulse</t>
+  </si>
+  <si>
+    <t>mm/encoder pulse</t>
+  </si>
+  <si>
+    <t>um/encoder pulse</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>100 pulses=1rev</t>
+  </si>
+  <si>
+    <t>rps</t>
+  </si>
+  <si>
+    <t>rev/sec</t>
+  </si>
+  <si>
+    <t>mm/sec</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>100ms</t>
+  </si>
+  <si>
+    <t>10ms</t>
+  </si>
+  <si>
+    <t>1ms</t>
+  </si>
+  <si>
+    <t>.1ms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,8 +179,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3611,7 +3695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE9D427-C038-416B-B3CB-C49351CC73FA}">
   <dimension ref="O20:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
@@ -3661,4 +3745,241 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A985047F-B597-4258-A3B5-C4A682226A0B}">
+  <dimension ref="B4:C4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21480089-8C8A-495B-9CCF-B137372E0229}">
+  <dimension ref="A2:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <f>13*25.4</f>
+        <v>330.2</v>
+      </c>
+      <c r="E3">
+        <f>D3*1000</f>
+        <v>330200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <f>3.14159*D3</f>
+        <v>1037.353018</v>
+      </c>
+      <c r="E5">
+        <f>D5*1000</f>
+        <v>1037353.018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>354</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <v>0.1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <f>(D5/B7)/B8</f>
+        <v>2.930375757062147E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f>D9*1000</f>
+        <v>29.303757570621471</v>
+      </c>
+      <c r="I9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11">
+        <v>100</v>
+      </c>
+      <c r="K11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>1E-4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <f>B12</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F12">
+        <f>(F9*0.000001)/D12</f>
+        <v>0.29303757570621469</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <f>B12*100</f>
+        <v>0.01</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <f>1/B13</f>
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <f>D5*B14</f>
+        <v>103735.3018</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>B15/1000</f>
+        <v>103.7353018</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
V0.2.2  Pushed pins for MTR A/B
Moved Pins on Encoder and motor to remove DIR signal and change to MTRA and MTR B signal
</commit_message>
<xml_diff>
--- a/Block diagram.xlsx
+++ b/Block diagram.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave\Documents\pico-robo-wheels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECDB297-7A85-495E-8780-B61BA444BCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D3C079-3104-44E1-87B6-89B06E6C0158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="390" windowWidth="20490" windowHeight="10605" activeTab="4" xr2:uid="{991C9B8B-21B3-447E-81C5-65B03554A51A}"/>
+    <workbookView xWindow="-360" yWindow="510" windowWidth="20490" windowHeight="10605" activeTab="2" xr2:uid="{991C9B8B-21B3-447E-81C5-65B03554A51A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Shinlin Motor" sheetId="3" r:id="rId3"/>
-    <sheet name="Encoder calcs" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="wiring" sheetId="6" r:id="rId3"/>
+    <sheet name="Shinlin Motor" sheetId="3" r:id="rId4"/>
+    <sheet name="Encoder calcs" sheetId="4" r:id="rId5"/>
+    <sheet name="period to velocity" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>IRQ relative addressing</t>
   </si>
@@ -149,6 +150,9 @@
   <si>
     <t>um/us</t>
   </si>
+  <si>
+    <t>m/hr</t>
+  </si>
 </sst>
 </file>
 
@@ -221,6 +225,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Period to m/s</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -261,7 +290,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$2</c:f>
+              <c:f>'period to velocity'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -296,21 +325,21 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$C$3:$C$15</c:f>
+              <c:f>'period to velocity'!$C$3:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>51.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>51.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>100</c:v>
@@ -331,34 +360,34 @@
                   <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5000</c:v>
+                  <c:v>2510</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7500</c:v>
+                  <c:v>2510</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10000</c:v>
+                  <c:v>2510</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$D$3:$D$15</c:f>
+              <c:f>'period to velocity'!$D$3:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>12.7</c:v>
+                  <c:v>2.48046875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.08</c:v>
+                  <c:v>2.4853228962818004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.54</c:v>
+                  <c:v>2.4901960784313726</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6933333333333334</c:v>
+                  <c:v>2.54</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.27</c:v>
@@ -379,13 +408,13 @@
                   <c:v>5.0799999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5399999999999999E-2</c:v>
+                  <c:v>5.0597609561752986E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.6933333333333335E-2</c:v>
+                  <c:v>5.0597609561752986E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.2699999999999999E-2</c:v>
+                  <c:v>5.0597609561752986E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4436,6 +4465,932 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C25480A2-3365-CA12-0311-2D265E30F154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5257800" y="390525"/>
+          <a:ext cx="7858125" cy="5267325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1362075" cy="323850"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{212016B3-1283-DC95-C942-A685ADDBA250}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4067174" y="828675"/>
+          <a:ext cx="1362075" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LeftPwmPin=1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1457325" cy="323850"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F89897E5-7DAE-4C61-BEA7-4B5401BBB5E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4048124" y="1304925"/>
+          <a:ext cx="1457325" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LeftMTRPinA =2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1476375" cy="323850"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66FF492D-61E9-49A4-85F4-959A7F21B3CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3933824" y="3086100"/>
+          <a:ext cx="1476375" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>RightPwmPin=8</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1476375" cy="323850"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDA5D636-00FC-4F04-9D22-5FF9BC3F34A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3933824" y="3305175"/>
+          <a:ext cx="1476375" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>RightMtrPinA=9</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1457325" cy="323850"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F32E082B-EB14-400A-9482-C5EE4412F93D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4095749" y="1866900"/>
+          <a:ext cx="1457325" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LeftENCA =4</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1457325" cy="323850"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32E213B5-E160-43C8-B75A-FDC6C1570DDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4086224" y="2066925"/>
+          <a:ext cx="1457325" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LeftENCB =5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1457325" cy="323850"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34F3BB30-46A6-43D8-9487-7F9D666A67B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4029074" y="2571750"/>
+          <a:ext cx="1457325" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>RightENCA =6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1457325" cy="323850"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{181AF877-B3D4-47A6-9E28-EBF7F91EBB58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4038599" y="2790825"/>
+          <a:ext cx="1457325" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>RightENCB =7</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1457325" cy="323850"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DE51A5E-4044-4B1A-8503-F1D021C56091}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4048124" y="1562100"/>
+          <a:ext cx="1457325" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LeftMTRPinB =3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1476375" cy="323850"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFC0C84E-BA74-4940-8B2C-65C678467345}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3933824" y="3810000"/>
+          <a:ext cx="1476375" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>RightMtrPinA=10</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -4809,7 +5764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE9D427-C038-416B-B3CB-C49351CC73FA}">
   <dimension ref="O20:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
@@ -4862,6 +5817,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8234F56-C959-499D-B251-0C507C06CF3A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A985047F-B597-4258-A3B5-C4A682226A0B}">
   <dimension ref="B4:C4"/>
   <sheetViews>
@@ -4884,7 +5854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21480089-8C8A-495B-9CCF-B137372E0229}">
   <dimension ref="A2:K16"/>
   <sheetViews>
@@ -5098,17 +6068,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47CA71-ADD7-44A9-BE58-6EBE58C05B10}">
-  <dimension ref="B2:D15"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>35</v>
       </c>
@@ -5118,56 +6088,75 @@
       <c r="D2" t="s">
         <v>29</v>
       </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>127</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>51.2</v>
       </c>
       <c r="D3">
         <f>B3/C3</f>
-        <v>12.7</v>
+        <v>2.48046875</v>
+      </c>
+      <c r="E3">
+        <f>D3*2.24</f>
+        <v>5.5562500000000004</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>127</v>
       </c>
       <c r="C4">
-        <v>25</v>
+        <v>51.1</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D6" si="0">B4/C4</f>
-        <v>5.08</v>
+        <v>2.4853228962818004</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E15" si="1">D4*2.24</f>
+        <v>5.5671232876712331</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>127</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>2.54</v>
+        <v>2.4901960784313726</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>5.5780392156862755</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>127</v>
       </c>
       <c r="C6">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>1.6933333333333334</v>
+        <v>2.54</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>5.6896000000000004</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>127</v>
       </c>
@@ -5178,8 +6167,12 @@
         <f>B7/C7</f>
         <v>1.27</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>2.8448000000000002</v>
+      </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>127</v>
       </c>
@@ -5187,11 +6180,15 @@
         <v>250</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D10" si="1">B8/C8</f>
+        <f t="shared" ref="D8:D10" si="2">B8/C8</f>
         <v>0.50800000000000001</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>1.13792</v>
+      </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>127</v>
       </c>
@@ -5199,11 +6196,15 @@
         <v>500</v>
       </c>
       <c r="D9">
+        <f t="shared" si="2"/>
+        <v>0.254</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="1"/>
-        <v>0.254</v>
+        <v>0.56896000000000002</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>127</v>
       </c>
@@ -5211,11 +6212,15 @@
         <v>750</v>
       </c>
       <c r="D10">
+        <f t="shared" si="2"/>
+        <v>0.16933333333333334</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="1"/>
-        <v>0.16933333333333334</v>
+        <v>0.37930666666666668</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>127</v>
       </c>
@@ -5226,8 +6231,12 @@
         <f>B11/C11</f>
         <v>0.127</v>
       </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.28448000000000001</v>
+      </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>127</v>
       </c>
@@ -5238,41 +6247,57 @@
         <f>B12/C12</f>
         <v>5.0799999999999998E-2</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0.113792</v>
+      </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>127</v>
       </c>
       <c r="C13">
-        <v>5000</v>
+        <v>2510</v>
       </c>
       <c r="D13">
         <f>B13/C13</f>
-        <v>2.5399999999999999E-2</v>
+        <v>5.0597609561752986E-2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0.11333864541832669</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>127</v>
       </c>
       <c r="C14">
-        <v>7500</v>
+        <v>2510</v>
       </c>
       <c r="D14">
         <f>B14/C14</f>
-        <v>1.6933333333333335E-2</v>
+        <v>5.0597609561752986E-2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0.11333864541832669</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>127</v>
       </c>
       <c r="C15">
-        <v>10000</v>
+        <v>2510</v>
       </c>
       <c r="D15">
         <f>B15/C15</f>
-        <v>1.2699999999999999E-2</v>
+        <v>5.0597609561752986E-2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0.11333864541832669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cmds, mtr dir
added FW,RT,LT,ST,TV, and PW cmds
</commit_message>
<xml_diff>
--- a/Block diagram.xlsx
+++ b/Block diagram.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave\Documents\pico-robo-wheels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D3C079-3104-44E1-87B6-89B06E6C0158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF74473A-3CBC-4240-B5BC-4AD77C8D87DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-360" yWindow="510" windowWidth="20490" windowHeight="10605" activeTab="2" xr2:uid="{991C9B8B-21B3-447E-81C5-65B03554A51A}"/>
+    <workbookView xWindow="195" yWindow="375" windowWidth="20490" windowHeight="10605" activeTab="4" xr2:uid="{991C9B8B-21B3-447E-81C5-65B03554A51A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="wiring" sheetId="6" r:id="rId3"/>
-    <sheet name="Shinlin Motor" sheetId="3" r:id="rId4"/>
-    <sheet name="Encoder calcs" sheetId="4" r:id="rId5"/>
-    <sheet name="period to velocity" sheetId="5" r:id="rId6"/>
+    <sheet name="Battery Specs" sheetId="7" r:id="rId4"/>
+    <sheet name="100A Driver" sheetId="8" r:id="rId5"/>
+    <sheet name="Shinlin Motor" sheetId="3" r:id="rId6"/>
+    <sheet name="Encoder calcs" sheetId="4" r:id="rId7"/>
+    <sheet name="period to velocity" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>IRQ relative addressing</t>
   </si>
@@ -153,6 +155,48 @@
   <si>
     <t>m/hr</t>
   </si>
+  <si>
+    <t>Brand new in the original boxes. Crazy deal on these.</t>
+  </si>
+  <si>
+    <t>Max Continuous Charge Rate - 67a</t>
+  </si>
+  <si>
+    <t>Max Continuous Discharge Rate - 450a (high power)</t>
+  </si>
+  <si>
+    <t>These use Samsung 67ah prismatic power cells.</t>
+  </si>
+  <si>
+    <t>They were overstock and came in the original pallets.</t>
+  </si>
+  <si>
+    <t>You can easily add an 8s Lithium Ion BMS since the balance leads are already connected, simply connect the balance leads to your BMS. The board you see on the front is just a balancer and communication pcb but that part is not a BMS, it just communicates to another main BMS units. So you will have the add your own BMS which would be super easy as you can see in the photos. The case just pops right off if you use a flat screw driver.</t>
+  </si>
+  <si>
+    <t>The modules are also light enough to ship ground instead of freight which is a huge bonus. They are 8s lithium ion with a 3.8 nominal voltage per cell and 67ah. You can expect high cycle life out of the cells since they are EV grade Samsung cells. Each cell fully charged voltage is 4.2v and fully discharged is 2.8v. The cells are in 8s configuration.</t>
+  </si>
+  <si>
+    <t>Check the 2nd photo for the specs.</t>
+  </si>
+  <si>
+    <t>Dimensions are 16.5" x 9" x 7"</t>
+  </si>
+  <si>
+    <t>Module Fully charged 33.6v</t>
+  </si>
+  <si>
+    <t>Module Fully Discharged 22.4v</t>
+  </si>
+  <si>
+    <t>Main +/- bolt size: M8 x 1.25</t>
+  </si>
+  <si>
+    <t>Weight 37 lbs</t>
+  </si>
+  <si>
+    <t>Note: Some are all black and some are black/grey. We will send you all the same color. They are both the same battery, just one has the positive post on the right and the other has it on the left.</t>
+  </si>
 </sst>
 </file>
 
@@ -161,13 +205,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,9 +240,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5391,6 +5447,280 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>601690</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>67482</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D706529A-7B3E-71A6-3C75-26FCA3E5C083}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9077325" y="190500"/>
+          <a:ext cx="11574490" cy="5782482"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>506917</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>637</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8F05CDE-55C8-C54A-3871-02F48D2199DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="542924"/>
+          <a:ext cx="4774116" cy="4220213"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>27215</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>24493</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>515698</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>136832</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F58D680A-4792-6629-299A-43CBF9996685}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8912679" y="595993"/>
+          <a:ext cx="9673305" cy="5446339"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>421821</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>303437</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>181519</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BFB59FB-3A1D-123E-6549-2C2ADB3A4047}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5279571" y="6191250"/>
+          <a:ext cx="9735909" cy="3896269"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>449035</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>51751</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>108131</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A248E9D2-D274-F1C6-4517-E6B98902D540}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5306785" y="10423072"/>
+          <a:ext cx="10069330" cy="4544059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>544664</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>38545</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6170B259-E2FE-1961-5B26-2C206C2F4534}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6067425"/>
+          <a:ext cx="5383364" cy="2543620"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -5820,7 +6150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8234F56-C959-499D-B251-0C507C06CF3A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -5832,6 +6162,191 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3D5C52-FC70-42E4-9AF0-6EB240E9C020}">
+  <dimension ref="B3:B41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="117.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D99EF5FE-145F-4222-94FB-064C1665CDDE}">
+  <dimension ref="I1:J1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K32" sqref="K1:K1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A985047F-B597-4258-A3B5-C4A682226A0B}">
   <dimension ref="B4:C4"/>
   <sheetViews>
@@ -5854,7 +6369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21480089-8C8A-495B-9CCF-B137372E0229}">
   <dimension ref="A2:K16"/>
   <sheetViews>
@@ -6068,7 +6583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C47CA71-ADD7-44A9-BE58-6EBE58C05B10}">
   <dimension ref="B2:E15"/>
   <sheetViews>

</xml_diff>